<commit_message>
change in condition labelling
</commit_message>
<xml_diff>
--- a/exploration proposal_power.xlsx
+++ b/exploration proposal_power.xlsx
@@ -93,12 +93,6 @@
     <t>proportion looking time to unseen space</t>
   </si>
   <si>
-    <t>no-toy / neutral: 0.2</t>
-  </si>
-  <si>
-    <t>toy / emotional: 0.4</t>
-  </si>
-  <si>
     <t>glm(resp~condition + sex +z.age, family=beta)</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 5/6</t>
+  </si>
+  <si>
+    <t>no-toy / control: 0.2</t>
+  </si>
+  <si>
+    <t>toy / positive: 0.4</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
@@ -570,16 +570,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F2">
         <v>350</v>
@@ -594,10 +594,10 @@
         <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -611,10 +611,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -632,7 +632,7 @@
         <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -646,10 +646,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1">
         <v>68</v>
@@ -675,10 +675,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1">
         <v>48</v>
@@ -698,16 +698,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1">
         <v>68</v>
@@ -719,15 +719,15 @@
         <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -736,10 +736,10 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="G7" s="1">
         <v>32</v>
@@ -751,7 +751,7 @@
         <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -782,10 +782,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.45">
@@ -793,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1">
         <v>20</v>
@@ -805,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>68</v>
@@ -819,7 +819,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
         <v>68</v>
@@ -833,7 +833,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1">
         <v>68</v>
@@ -845,7 +845,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>68</v>
@@ -857,13 +857,13 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1">
         <v>30</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
@@ -871,7 +871,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1">
         <v>30</v>

</xml_diff>